<commit_message>
Add functionality to download consolidated invoices via API
Update server/routes.ts to include file download logic for consolidated invoices, removing redundant require statements for fs and path.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ec732b10-5df2-4b3f-a5f6-e0d4f648d70f
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4cf1d16a-ee39-486f-884d-afb5e948f672/ec732b10-5df2-4b3f-a5f6-e0d4f648d70f/88umdma
</commit_message>
<xml_diff>
--- a/python_backend/output/Consolidated_Invoices_Output.xlsx
+++ b/python_backend/output/Consolidated_Invoices_Output.xlsx
@@ -49,9 +49,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -417,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -489,6 +492,65 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>WESTSIDE
+Sjr Zion, Survey</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>29AAACL1838J1ZC</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>W089100169940</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2024-09-28</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>4045.01</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>173.91</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>173.91</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>173.91</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J2" s="2" t="inlineStr">
+        <is>
+          <t>996211
+62052000
+62052000
+62046200
+48194000
+33072000
+39264099</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add download history tracking and display to the platform
Integrate download history logging into the Excel download endpoint and create a new API endpoint and frontend component to display this history.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ec732b10-5df2-4b3f-a5f6-e0d4f648d70f
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4cf1d16a-ee39-486f-884d-afb5e948f672/ec732b10-5df2-4b3f-a5f6-e0d4f648d70f/Zy7Dkib
</commit_message>
<xml_diff>
--- a/python_backend/output/Consolidated_Invoices_Output.xlsx
+++ b/python_backend/output/Consolidated_Invoices_Output.xlsx
@@ -495,8 +495,8 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>WESTSIDE
-Sjr Zion, Survey</t>
+          <t xml:space="preserve">Westside
+</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -542,12 +542,12 @@
       <c r="J2" s="2" t="inlineStr">
         <is>
           <t>996211
-62052000
-62052000
-62046200
-48194000
-33072000
-39264099</t>
+300980061004
+300988526002
+300992658003
+600000562
+300922355001
+300989351001</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update website to a professional, dynamic, and secure enterprise application
Refactor the application to remove gradients, implement a new navigation system with dedicated pages for GST returns, analytics, and reports, incorporate Indian GST compliance features, and introduce a professional logo and branding.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ec732b10-5df2-4b3f-a5f6-e0d4f648d70f
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4cf1d16a-ee39-486f-884d-afb5e948f672/ec732b10-5df2-4b3f-a5f6-e0d4f648d70f/DssZMve
</commit_message>
<xml_diff>
--- a/python_backend/output/Consolidated_Invoices_Output.xlsx
+++ b/python_backend/output/Consolidated_Invoices_Output.xlsx
@@ -495,8 +495,8 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Westside
-</t>
+          <t>WESTSIDE
+UNIT OF TRENT LTD</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -506,7 +506,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>W089100169940</t>
+          <t>W089 100169940</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">

</xml_diff>

<commit_message>
Enhance user experience with a streamlined authentication flow and improved report management
Integrate "login with Replit" functionality, refactor authentication hooks for better data handling, introduce toast notifications for user feedback, implement report deletion with backend support, and update the logo component with professional styling. Also, update dependencies for enhanced functionality.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ec732b10-5df2-4b3f-a5f6-e0d4f648d70f
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4cf1d16a-ee39-486f-884d-afb5e948f672/ec732b10-5df2-4b3f-a5f6-e0d4f648d70f/fOz65qX
</commit_message>
<xml_diff>
--- a/python_backend/output/Consolidated_Invoices_Output.xlsx
+++ b/python_backend/output/Consolidated_Invoices_Output.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,43 +495,43 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>WESTSIDE
-UNIT OF TRENT LTD</t>
+          <t>SONOVISION ELECTRONICS
+PVT LTD</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>29AAACL1838J1ZC</t>
+          <t>37ABCCS7530B1ZK</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>W089 100169940</t>
+          <t>NDYL 3826</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2024-09-28</t>
+          <t>17/Feb/2023</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>4045.01</t>
+          <t>69000</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>173.91</t>
+          <t>15094</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>173.91</t>
+          <t>7547</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>173.91</t>
+          <t>7547</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -541,13 +541,66 @@
       </c>
       <c r="J2" s="2" t="inlineStr">
         <is>
-          <t>996211
-300980061004
-300988526002
-300992658003
-600000562
-300922355001
-300989351001</t>
+          <t>85287219
+0</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>LAKSHMI AGENCIES
+No:18, Kannadasan Nagar Main Road,
+Ramapuram</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>33AABFL7718B1ZQ</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>LA226412507098</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>17/07/2025</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>33725.00</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>1440.00</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>720.00</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>720.00</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J3" s="2" t="inlineStr">
+        <is>
+          <t>15121910
+15121910
+15121910
+15180039
+15180039</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix incorrect redirection to the compliance page by displaying the actual compliance content.
Update the route for "/compliance" in `App.tsx` to render `CompliancePage` instead of `DashboardPage`.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 85863112-a031-405a-83ae-302c869661f0
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/a76d741b-8ad6-464e-a09a-fc6953be1e99/85863112-a031-405a-83ae-302c869661f0/Gq0zFN1
</commit_message>
<xml_diff>
--- a/python_backend/output/Consolidated_Invoices_Output.xlsx
+++ b/python_backend/output/Consolidated_Invoices_Output.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,43 +495,43 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>SONOVISION ELECTRONICS
-PVT LTD</t>
+          <t>WESTSIDE
+Sjr Zion, Survey</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>37ABCCS7530B1ZK</t>
+          <t>29AAACL1838J1ZC</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>NDYL 3826</t>
+          <t>W089 100169940</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>17/Feb/2023</t>
+          <t>2024-09-28</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>69000</t>
+          <t>4045.01</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>15094</t>
+          <t>173.91</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>7547</t>
+          <t>173.91</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>7547</t>
+          <t>173.91</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -541,66 +541,13 @@
       </c>
       <c r="J2" s="2" t="inlineStr">
         <is>
-          <t>85287219
-0</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>LAKSHMI AGENCIES
-No:18, Kannadasan Nagar Main Road,
-Ramapuram</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>33AABFL7718B1ZQ</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>LA226412507098</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>17/07/2025</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>33725.00</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>1440.00</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>720.00</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>720.00</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="J3" s="2" t="inlineStr">
-        <is>
-          <t>15121910
-15121910
-15121910
-15180039
-15180039</t>
+          <t>0
+62052000
+62052000
+62046200
+48194000
+33072000
+39264099</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Simplify GST report formatting by removing colors and complex styling
Remove all styling, borders, and coloring from the GST report generation in `writer_agent.py`, simplifying the output to a structured format as requested.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 85863112-a031-405a-83ae-302c869661f0
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/a76d741b-8ad6-464e-a09a-fc6953be1e99/85863112-a031-405a-83ae-302c869661f0/XbWxbdl
</commit_message>
<xml_diff>
--- a/python_backend/output/Consolidated_Invoices_Output.xlsx
+++ b/python_backend/output/Consolidated_Invoices_Output.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="GST Report" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="GST Audit Report" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -26,18 +26,45 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Arial"/>
       <b val="1"/>
+      <color rgb="00FFFFFF"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <b val="1"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <i val="1"/>
+      <sz val="9"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="9"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="002B5D84"/>
+        <bgColor rgb="002B5D84"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -45,16 +72,68 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -420,138 +499,194 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="18" customWidth="1" min="1" max="1"/>
-    <col width="18" customWidth="1" min="2" max="2"/>
+    <col width="8" customWidth="1" min="1" max="1"/>
+    <col width="25" customWidth="1" min="2" max="2"/>
     <col width="18" customWidth="1" min="3" max="3"/>
-    <col width="18" customWidth="1" min="4" max="4"/>
-    <col width="18" customWidth="1" min="5" max="5"/>
-    <col width="18" customWidth="1" min="6" max="6"/>
-    <col width="18" customWidth="1" min="7" max="7"/>
-    <col width="18" customWidth="1" min="8" max="8"/>
-    <col width="18" customWidth="1" min="9" max="9"/>
-    <col width="30" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
+    <col width="12" customWidth="1" min="8" max="8"/>
+    <col width="12" customWidth="1" min="9" max="9"/>
+    <col width="12" customWidth="1" min="10" max="10"/>
+    <col width="35" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="30" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Shop Name</t>
+          <t>S.No.</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Vendor/Shop Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>GSTIN</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Invoice Number</t>
-        </is>
-      </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Invoice Date</t>
+          <t>Invoice No.</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Total Amount</t>
+          <t>Date</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Tax Amount</t>
+          <t>Taxable Amount</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>Total Tax</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>CGST</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>SGST</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>IGST</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>HSN Code</t>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>HSN Codes</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>WESTSIDE
-Sjr Zion, Survey</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
+    <row r="2" ht="25" customHeight="1">
+      <c r="A2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>WESTSIDE, Sjr Zion, Survey</t>
+        </is>
+      </c>
+      <c r="C2" s="4" t="inlineStr">
         <is>
           <t>29AAACL1838J1ZC</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" s="4" t="inlineStr">
         <is>
           <t>W089 100169940</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" s="4" t="inlineStr">
         <is>
           <t>2024-09-28</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" s="4" t="inlineStr">
         <is>
           <t>4045.01</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" s="4" t="inlineStr">
         <is>
           <t>173.91</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" s="4" t="inlineStr">
         <is>
           <t>173.91</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" s="4" t="inlineStr">
         <is>
           <t>173.91</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" s="4" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="J2" s="2" t="inlineStr">
-        <is>
-          <t>996211
-62052000
-62052000
-62046200
-48194000
-33072000
-39264099</t>
+      <c r="K2" s="3" t="inlineStr">
+        <is>
+          <t>996211, 62052000, 62052000, 62046200, 48194000, 33072000, 39264099</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+      <c r="B3" s="6" t="n"/>
+      <c r="C3" s="6" t="n"/>
+      <c r="D3" s="6" t="n"/>
+      <c r="E3" s="7" t="n"/>
+      <c r="F3" s="8" t="inlineStr">
+        <is>
+          <t>₹4,045.01</t>
+        </is>
+      </c>
+      <c r="G3" s="8" t="inlineStr">
+        <is>
+          <t>₹173.91</t>
+        </is>
+      </c>
+      <c r="H3" s="8" t="inlineStr">
+        <is>
+          <t>₹173.91</t>
+        </is>
+      </c>
+      <c r="I3" s="8" t="inlineStr">
+        <is>
+          <t>₹173.91</t>
+        </is>
+      </c>
+      <c r="J3" s="8" t="inlineStr">
+        <is>
+          <t>₹0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="9" t="inlineStr">
+        <is>
+          <t>Generated for GST Audit Purposes</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="10" t="inlineStr">
+        <is>
+          <t>Total Invoices: 1</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A3:E3"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add GST-compliant Excel report generation with detailed invoice fields
Update the Excel report generation to include a B2B Invoices sheet with expanded fields, supplier information, tax breakdowns, and other GST-required data.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 85863112-a031-405a-83ae-302c869661f0
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/a76d741b-8ad6-464e-a09a-fc6953be1e99/85863112-a031-405a-83ae-302c869661f0/MxWl5C1
</commit_message>
<xml_diff>
--- a/python_backend/output/Consolidated_Invoices_Output.xlsx
+++ b/python_backend/output/Consolidated_Invoices_Output.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="GST Audit Report" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="GST Report" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -25,46 +25,16 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <name val="Arial"/>
-      <b val="1"/>
-      <color rgb="00FFFFFF"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <b val="1"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <i val="1"/>
-      <sz val="9"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="9"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="002B5D84"/>
-        <bgColor rgb="002B5D84"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="6">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -72,68 +42,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -499,11 +413,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -521,172 +434,119 @@
     <col width="35" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
-    <row r="1" ht="30" customHeight="1">
-      <c r="A1" s="1" t="inlineStr">
+    <row r="1">
+      <c r="A1" t="inlineStr">
         <is>
           <t>S.No.</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>Vendor/Shop Name</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>GSTIN</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>Invoice No.</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>Taxable Amount</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>Total Tax</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>CGST</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>SGST</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>IGST</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>HSN Codes</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="25" customHeight="1">
-      <c r="A2" s="2" t="n">
+    <row r="2">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
           <t>WESTSIDE, Sjr Zion, Survey</t>
         </is>
       </c>
-      <c r="C2" s="4" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>29AAACL1838J1ZC</t>
         </is>
       </c>
-      <c r="D2" s="4" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>W089 100169940</t>
         </is>
       </c>
-      <c r="E2" s="4" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>2024-09-28</t>
         </is>
       </c>
-      <c r="F2" s="4" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>4045.01</t>
         </is>
       </c>
-      <c r="G2" s="4" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>173.91</t>
         </is>
       </c>
-      <c r="H2" s="4" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>173.91</t>
         </is>
       </c>
-      <c r="I2" s="4" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>173.91</t>
         </is>
       </c>
-      <c r="J2" s="4" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="K2" s="3" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>996211, 62052000, 62052000, 62046200, 48194000, 33072000, 39264099</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="5" t="inlineStr">
-        <is>
-          <t>TOTAL</t>
-        </is>
-      </c>
-      <c r="B3" s="6" t="n"/>
-      <c r="C3" s="6" t="n"/>
-      <c r="D3" s="6" t="n"/>
-      <c r="E3" s="7" t="n"/>
-      <c r="F3" s="8" t="inlineStr">
-        <is>
-          <t>₹4,045.01</t>
-        </is>
-      </c>
-      <c r="G3" s="8" t="inlineStr">
-        <is>
-          <t>₹173.91</t>
-        </is>
-      </c>
-      <c r="H3" s="8" t="inlineStr">
-        <is>
-          <t>₹173.91</t>
-        </is>
-      </c>
-      <c r="I3" s="8" t="inlineStr">
-        <is>
-          <t>₹173.91</t>
-        </is>
-      </c>
-      <c r="J3" s="8" t="inlineStr">
-        <is>
-          <t>₹0.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="9" t="inlineStr">
-        <is>
-          <t>Generated for GST Audit Purposes</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="10" t="inlineStr">
-        <is>
-          <t>Total Invoices: 1</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A3:E3"/>
-  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Saved your changes before starting work
Replit-Commit-Author: Agent
Replit-Commit-Session-Id: a28a4f51-f475-4328-a54d-afd84476b9d9
Replit-Commit-Checkpoint-Type: full_checkpoint
</commit_message>
<xml_diff>
--- a/python_backend/output/Consolidated_Invoices_Output.xlsx
+++ b/python_backend/output/Consolidated_Invoices_Output.xlsx
@@ -7,7 +7,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="GST Report" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="B2B Invoices" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="HSN Summary" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Document Issued" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -421,17 +423,30 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="8" customWidth="1" min="1" max="1"/>
-    <col width="25" customWidth="1" min="2" max="2"/>
-    <col width="18" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
-    <col width="12" customWidth="1" min="5" max="5"/>
-    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="6" customWidth="1" min="1" max="1"/>
+    <col width="18" customWidth="1" min="2" max="2"/>
+    <col width="25" customWidth="1" min="3" max="3"/>
+    <col width="30" customWidth="1" min="4" max="4"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
     <col width="12" customWidth="1" min="7" max="7"/>
-    <col width="12" customWidth="1" min="8" max="8"/>
-    <col width="12" customWidth="1" min="9" max="9"/>
+    <col width="15" customWidth="1" min="8" max="8"/>
+    <col width="20" customWidth="1" min="9" max="9"/>
     <col width="12" customWidth="1" min="10" max="10"/>
-    <col width="35" customWidth="1" min="11" max="11"/>
+    <col width="12" customWidth="1" min="11" max="11"/>
+    <col width="10" customWidth="1" min="12" max="12"/>
+    <col width="25" customWidth="1" min="13" max="13"/>
+    <col width="10" customWidth="1" min="14" max="14"/>
+    <col width="8" customWidth="1" min="15" max="15"/>
+    <col width="12" customWidth="1" min="16" max="16"/>
+    <col width="15" customWidth="1" min="17" max="17"/>
+    <col width="10" customWidth="1" min="18" max="18"/>
+    <col width="12" customWidth="1" min="19" max="19"/>
+    <col width="12" customWidth="1" min="20" max="20"/>
+    <col width="12" customWidth="1" min="21" max="21"/>
+    <col width="12" customWidth="1" min="22" max="22"/>
+    <col width="12" customWidth="1" min="23" max="23"/>
+    <col width="15" customWidth="1" min="24" max="24"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -442,52 +457,117 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Vendor/Shop Name</t>
+          <t>Recipient GSTIN</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>GSTIN</t>
+          <t>Supplier Name</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Invoice No.</t>
+          <t>Supplier Address</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Date</t>
+          <t>Supplier GSTIN</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>Taxable Amount</t>
+          <t>Invoice Number</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>Total Tax</t>
+          <t>Invoice Date</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>CGST</t>
+          <t>Invoice Value</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>SGST</t>
+          <t>Place of Supply</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>IGST</t>
+          <t>Reverse Charge</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>HSN Codes</t>
+          <t>Invoice Type</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>HSN Code</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Item Description</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>Unit Code (UQC)</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>Unit Rate</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>Taxable Value</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>Tax Rate (%)</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>CGST Amount</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>SGST Amount</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>IGST Amount</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>UTGST Amount</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>Cess Amount</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>Discount/Abatement</t>
         </is>
       </c>
     </row>
@@ -495,54 +575,397 @@
       <c r="A2" t="n">
         <v>1</v>
       </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>WESTSIDE, Sjr Zion, Survey</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>29AAACL1838J1ZC</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>W089 100169940</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2024-09-28</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>4045.01</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>996211</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>4045.01</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>173.91</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>173.91</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
+      <c r="X2" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="6" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="30" customWidth="1" min="3" max="3"/>
+    <col width="8" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="10" customWidth="1" min="8" max="8"/>
+    <col width="12" customWidth="1" min="9" max="9"/>
+    <col width="12" customWidth="1" min="10" max="10"/>
+    <col width="12" customWidth="1" min="11" max="11"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>S.No.</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>HSN Code</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>UQC</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Total Quantity</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Total Value</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Taxable Value</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Tax Rate (%)</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>CGST Amount</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>SGST Amount</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>IGST Amount</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>WESTSIDE, Sjr Zion, Survey</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>29AAACL1838J1ZC</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>W089 100169940</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>2024-09-28</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>4045.01</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>173.91</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>173.91</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>173.91</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>996211, 62052000, 62052000, 62046200, 48194000, 33072000, 39264099</t>
+          <t>996211</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="n">
+        <v>40004050.0001</v>
+      </c>
+      <c r="G2" t="n">
+        <v>40004050.0001</v>
+      </c>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="n">
+        <v>107030.0901</v>
+      </c>
+      <c r="J2" t="n">
+        <v>107030.0901</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>62052000</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="n">
+        <v>80008100.0002</v>
+      </c>
+      <c r="G3" t="n">
+        <v>80008100.0002</v>
+      </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="n">
+        <v>214060.1802</v>
+      </c>
+      <c r="J3" t="n">
+        <v>214060.1802</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>62046200</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="n">
+        <v>40004050.0001</v>
+      </c>
+      <c r="G4" t="n">
+        <v>40004050.0001</v>
+      </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="n">
+        <v>107030.0901</v>
+      </c>
+      <c r="J4" t="n">
+        <v>107030.0901</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>48194000</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="n">
+        <v>40004050.0001</v>
+      </c>
+      <c r="G5" t="n">
+        <v>40004050.0001</v>
+      </c>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="n">
+        <v>107030.0901</v>
+      </c>
+      <c r="J5" t="n">
+        <v>107030.0901</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>33072000</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="n">
+        <v>40004050.0001</v>
+      </c>
+      <c r="G6" t="n">
+        <v>40004050.0001</v>
+      </c>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="n">
+        <v>107030.0901</v>
+      </c>
+      <c r="J6" t="n">
+        <v>107030.0901</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>39264099</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="n">
+        <v>40004050.0001</v>
+      </c>
+      <c r="G7" t="n">
+        <v>40004050.0001</v>
+      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="n">
+        <v>107030.0901</v>
+      </c>
+      <c r="J7" t="n">
+        <v>107030.0901</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>S.No.</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Document Type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Document Number From</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Document Number To</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Total Number</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Cancelled</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Improve Excel formatting for vendor names and HSN codes
Adjust column widths and apply text wrapping to cells for better display of vendor names and HSN codes in generated Excel reports, ensuring a more structured format.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: a28a4f51-f475-4328-a54d-afd84476b9d9
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/a76d741b-8ad6-464e-a09a-fc6953be1e99/a28a4f51-f475-4328-a54d-afd84476b9d9/XMRzFQk
</commit_message>
<xml_diff>
--- a/python_backend/output/Consolidated_Invoices_Output.xlsx
+++ b/python_backend/output/Consolidated_Invoices_Output.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="GST Audit Report" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="GST Report" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -25,46 +25,16 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <name val="Arial"/>
-      <b val="1"/>
-      <color rgb="00FFFFFF"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <b val="1"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <i val="1"/>
-      <sz val="9"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="9"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="002B5D84"/>
-        <bgColor rgb="002B5D84"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="6">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -72,68 +42,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -499,11 +413,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -521,172 +434,119 @@
     <col width="35" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
-    <row r="1" ht="30" customHeight="1">
-      <c r="A1" s="1" t="inlineStr">
+    <row r="1">
+      <c r="A1" t="inlineStr">
         <is>
           <t>S.No.</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>Vendor/Shop Name</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>GSTIN</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>Invoice No.</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>Taxable Amount</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>Total Tax</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>CGST</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>SGST</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>IGST</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>HSN Codes</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="25" customHeight="1">
-      <c r="A2" s="2" t="n">
+    <row r="2">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="inlineStr">
-        <is>
-          <t>WESTSIDE, Sjr Zion, Survey</t>
-        </is>
-      </c>
-      <c r="C2" s="4" t="inlineStr">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>WESTSIDE, A UNIT OF TRENT LTD</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
         <is>
           <t>29AAACL1838J1ZC</t>
         </is>
       </c>
-      <c r="D2" s="4" t="inlineStr">
-        <is>
-          <t>W089 100169940</t>
-        </is>
-      </c>
-      <c r="E2" s="4" t="inlineStr">
-        <is>
-          <t>2024-09-28</t>
-        </is>
-      </c>
-      <c r="F2" s="4" t="inlineStr">
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>W089100169940</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2024-09-28 17:41:22</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
         <is>
           <t>4045.01</t>
         </is>
       </c>
-      <c r="G2" s="4" t="inlineStr">
-        <is>
-          <t>173.91</t>
-        </is>
-      </c>
-      <c r="H2" s="4" t="inlineStr">
-        <is>
-          <t>173.91</t>
-        </is>
-      </c>
-      <c r="I2" s="4" t="inlineStr">
-        <is>
-          <t>173.91</t>
-        </is>
-      </c>
-      <c r="J2" s="4" t="inlineStr">
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>388.06</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>194.03</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>194.03</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="K2" s="3" t="inlineStr">
-        <is>
-          <t>996211, 62052000, 62052000, 62046200, 48194000, 33072000, 39264099</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="5" t="inlineStr">
-        <is>
-          <t>TOTAL</t>
-        </is>
-      </c>
-      <c r="B3" s="6" t="n"/>
-      <c r="C3" s="6" t="n"/>
-      <c r="D3" s="6" t="n"/>
-      <c r="E3" s="7" t="n"/>
-      <c r="F3" s="8" t="inlineStr">
-        <is>
-          <t>₹4,045.01</t>
-        </is>
-      </c>
-      <c r="G3" s="8" t="inlineStr">
-        <is>
-          <t>₹173.91</t>
-        </is>
-      </c>
-      <c r="H3" s="8" t="inlineStr">
-        <is>
-          <t>₹173.91</t>
-        </is>
-      </c>
-      <c r="I3" s="8" t="inlineStr">
-        <is>
-          <t>₹173.91</t>
-        </is>
-      </c>
-      <c r="J3" s="8" t="inlineStr">
-        <is>
-          <t>₹0.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="9" t="inlineStr">
-        <is>
-          <t>Generated for GST Audit Purposes</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="10" t="inlineStr">
-        <is>
-          <t>Total Invoices: 1</t>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>996211, 300980061004, 300988526002, 300992658003, 600000562, 300922355001, 300989351001</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A3:E3"/>
-  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update invoice report column order and widths
Modify the `writer_agent` function to reorder and adjust column widths in the generated Excel report to match the requested format. This includes changes to headers and cell alignment for improved readability.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: a28a4f51-f475-4328-a54d-afd84476b9d9
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/a76d741b-8ad6-464e-a09a-fc6953be1e99/a28a4f51-f475-4328-a54d-afd84476b9d9/u34HvdO
</commit_message>
<xml_diff>
--- a/python_backend/output/Consolidated_Invoices_Output.xlsx
+++ b/python_backend/output/Consolidated_Invoices_Output.xlsx
@@ -46,8 +46,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -422,19 +431,19 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="8" customWidth="1" min="1" max="1"/>
-    <col width="25" customWidth="1" min="2" max="2"/>
+    <col width="30" customWidth="1" min="2" max="2"/>
     <col width="18" customWidth="1" min="3" max="3"/>
     <col width="20" customWidth="1" min="4" max="4"/>
-    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="5" max="5"/>
     <col width="15" customWidth="1" min="6" max="6"/>
     <col width="12" customWidth="1" min="7" max="7"/>
     <col width="12" customWidth="1" min="8" max="8"/>
     <col width="12" customWidth="1" min="9" max="9"/>
     <col width="12" customWidth="1" min="10" max="10"/>
-    <col width="35" customWidth="1" min="11" max="11"/>
+    <col width="40" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="25" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
           <t>S.No.</t>
@@ -491,58 +500,58 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
+    <row r="2" ht="30" customHeight="1">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>WESTSIDE, A UNIT OF TRENT LTD</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>WESTSIDE Sjr Zion, Survey</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
         <is>
           <t>29AAACL1838J1ZC</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>W089100169940</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>2024-09-28 17:41:22</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
+      <c r="D2" s="3" t="inlineStr">
+        <is>
+          <t>W089 100169940</t>
+        </is>
+      </c>
+      <c r="E2" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-28</t>
+        </is>
+      </c>
+      <c r="F2" s="3" t="inlineStr">
         <is>
           <t>4045.01</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>388.06</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>194.03</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>194.03</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
+      <c r="G2" s="3" t="inlineStr">
+        <is>
+          <t>173.91</t>
+        </is>
+      </c>
+      <c r="H2" s="3" t="inlineStr">
+        <is>
+          <t>173.91</t>
+        </is>
+      </c>
+      <c r="I2" s="3" t="inlineStr">
+        <is>
+          <t>173.91</t>
+        </is>
+      </c>
+      <c r="J2" s="3" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>996211, 300980061004, 300988526002, 300992658003, 600000562, 300922355001, 300989351001</t>
+      <c r="K2" s="2" t="inlineStr">
+        <is>
+          <t>996211, 62052000, 62052000, 62046200, 48194000, 33072000, 39264099</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add functionality to upload generated Excel reports to the government portal
Introduces a new government upload page and integrates it into the application's navigation. The reports page now includes a button to navigate to the new government upload page. The new page simulates a government portal interface for uploading Excel files, including login, return selection, and file upload progress. The .replit file is updated to include the `javascript_object_storage` integration.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: a28a4f51-f475-4328-a54d-afd84476b9d9
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/a76d741b-8ad6-464e-a09a-fc6953be1e99/a28a4f51-f475-4328-a54d-afd84476b9d9/NrgzDH1
</commit_message>
<xml_diff>
--- a/python_backend/output/Consolidated_Invoices_Output.xlsx
+++ b/python_backend/output/Consolidated_Invoices_Output.xlsx
@@ -432,15 +432,15 @@
   <cols>
     <col width="8" customWidth="1" min="1" max="1"/>
     <col width="30" customWidth="1" min="2" max="2"/>
-    <col width="18" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="18" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="40" customWidth="1" min="6" max="6"/>
     <col width="12" customWidth="1" min="7" max="7"/>
     <col width="12" customWidth="1" min="8" max="8"/>
     <col width="12" customWidth="1" min="9" max="9"/>
     <col width="12" customWidth="1" min="10" max="10"/>
-    <col width="40" customWidth="1" min="11" max="11"/>
+    <col width="15" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1" ht="25" customHeight="1">
@@ -456,47 +456,47 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>GSTIN</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>Invoice No.</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>HSN Codes</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>CGST</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>SGST</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>IGST</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Total Tax</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
           <t>Taxable Amount</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>Total Tax</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>CGST</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>SGST</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>IGST</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>HSN Codes</t>
         </is>
       </c>
     </row>
@@ -511,47 +511,47 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
+          <t>2024-09-28</t>
+        </is>
+      </c>
+      <c r="D2" s="3" t="inlineStr">
+        <is>
           <t>29AAACL1838J1ZC</t>
         </is>
       </c>
-      <c r="D2" s="3" t="inlineStr">
+      <c r="E2" s="3" t="inlineStr">
         <is>
           <t>W089 100169940</t>
         </is>
       </c>
-      <c r="E2" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-28</t>
-        </is>
-      </c>
-      <c r="F2" s="3" t="inlineStr">
+      <c r="F2" s="2" t="inlineStr">
+        <is>
+          <t>996211, 62052000, 62052000, 62046200, 48194000, 33072000, 39264099</t>
+        </is>
+      </c>
+      <c r="G2" s="3" t="inlineStr">
+        <is>
+          <t>173.91</t>
+        </is>
+      </c>
+      <c r="H2" s="3" t="inlineStr">
+        <is>
+          <t>173.91</t>
+        </is>
+      </c>
+      <c r="I2" s="3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J2" s="3" t="inlineStr">
+        <is>
+          <t>173.91</t>
+        </is>
+      </c>
+      <c r="K2" s="3" t="inlineStr">
         <is>
           <t>4045.01</t>
-        </is>
-      </c>
-      <c r="G2" s="3" t="inlineStr">
-        <is>
-          <t>173.91</t>
-        </is>
-      </c>
-      <c r="H2" s="3" t="inlineStr">
-        <is>
-          <t>173.91</t>
-        </is>
-      </c>
-      <c r="I2" s="3" t="inlineStr">
-        <is>
-          <t>173.91</t>
-        </is>
-      </c>
-      <c r="J2" s="3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="K2" s="2" t="inlineStr">
-        <is>
-          <t>996211, 62052000, 62052000, 62046200, 48194000, 33072000, 39264099</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update report page to display logo correctly
Modify the `ReportsPage` component in `client/src/pages/reports.tsx` to change the text color of the report icon from blue to white.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: a28a4f51-f475-4328-a54d-afd84476b9d9
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/a76d741b-8ad6-464e-a09a-fc6953be1e99/a28a4f51-f475-4328-a54d-afd84476b9d9/k5Zsha7
</commit_message>
<xml_diff>
--- a/python_backend/output/Consolidated_Invoices_Output.xlsx
+++ b/python_backend/output/Consolidated_Invoices_Output.xlsx
@@ -506,7 +506,7 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>WESTSIDE Westside - Sjr Zion, Survey</t>
+          <t>WESTSIDE Sjr Zion, Survey</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr">
@@ -526,7 +526,7 @@
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>996211, 62052000, 62052000, 62046200, 48194000, 33072000, 39264099</t>
+          <t>996211, 300980061004, 300988526002, 300992658003, 600000562, 48194000, 33072000, 39264099</t>
         </is>
       </c>
       <c r="G2" s="3" t="inlineStr">

</xml_diff>

<commit_message>
Improve Excel cell formatting for multi-line text and HSN codes
Adjust column widths and cell alignment in the writer agent to properly display multi-line vendor names and HSN codes, while also refining HSN code extraction and formatting from item data.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: a28a4f51-f475-4328-a54d-afd84476b9d9
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/a76d741b-8ad6-464e-a09a-fc6953be1e99/a28a4f51-f475-4328-a54d-afd84476b9d9/nwgNhnr
</commit_message>
<xml_diff>
--- a/python_backend/output/Consolidated_Invoices_Output.xlsx
+++ b/python_backend/output/Consolidated_Invoices_Output.xlsx
@@ -422,7 +422,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -526,7 +526,7 @@
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>996211, 62052000, 62052000, 62046200, 48194000, 33072000, 39264099</t>
+          <t>996211, 300980061004, 300988526002, 300992658003, 600000562, 300922355001, 300989351001</t>
         </is>
       </c>
       <c r="G2" s="3" t="inlineStr">
@@ -552,6 +552,116 @@
       <c r="K2" s="3" t="inlineStr">
         <is>
           <t>4045.01</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="30" customHeight="1">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>SONOVISION ELECTRONICS PVT LTD</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>17/Feb/2023</t>
+        </is>
+      </c>
+      <c r="D3" s="3" t="inlineStr">
+        <is>
+          <t>37ABCCS7530B1ZK</t>
+        </is>
+      </c>
+      <c r="E3" s="3" t="inlineStr">
+        <is>
+          <t>NDYL 3826</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="inlineStr">
+        <is>
+          <t>85287219, 0</t>
+        </is>
+      </c>
+      <c r="G3" s="3" t="inlineStr">
+        <is>
+          <t>7547</t>
+        </is>
+      </c>
+      <c r="H3" s="3" t="inlineStr">
+        <is>
+          <t>7547</t>
+        </is>
+      </c>
+      <c r="I3" s="3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J3" s="3" t="inlineStr">
+        <is>
+          <t>15094</t>
+        </is>
+      </c>
+      <c r="K3" s="3" t="inlineStr">
+        <is>
+          <t>69000</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="30" customHeight="1">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>LAKSHMI AGENCIES No:18, Kannadasan Nagar Main Road, Ramapuram</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>17/07/2025</t>
+        </is>
+      </c>
+      <c r="D4" s="3" t="inlineStr">
+        <is>
+          <t>33AABFL7718B1ZQ</t>
+        </is>
+      </c>
+      <c r="E4" s="3" t="inlineStr">
+        <is>
+          <t>LA226412507098</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="inlineStr">
+        <is>
+          <t>15121910, 15121910, 15121910, 15180039, 15180039</t>
+        </is>
+      </c>
+      <c r="G4" s="3" t="inlineStr">
+        <is>
+          <t>720.00</t>
+        </is>
+      </c>
+      <c r="H4" s="3" t="inlineStr">
+        <is>
+          <t>720.00</t>
+        </is>
+      </c>
+      <c r="I4" s="3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J4" s="3" t="inlineStr">
+        <is>
+          <t>1913.39</t>
+        </is>
+      </c>
+      <c r="K4" s="3" t="inlineStr">
+        <is>
+          <t>33725.00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Improve Excel report formatting by centering all text within cells
Update the writer agent to apply horizontal and vertical centering to all data cells, including headers, to ensure consistent and aligned presentation in generated Excel reports.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: a28a4f51-f475-4328-a54d-afd84476b9d9
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/a76d741b-8ad6-464e-a09a-fc6953be1e99/a28a4f51-f475-4328-a54d-afd84476b9d9/Vz5gj9d
</commit_message>
<xml_diff>
--- a/python_backend/output/Consolidated_Invoices_Output.xlsx
+++ b/python_backend/output/Consolidated_Invoices_Output.xlsx
@@ -52,7 +52,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
@@ -431,11 +431,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="8" customWidth="1" min="1" max="1"/>
-    <col width="30" customWidth="1" min="2" max="2"/>
+    <col width="35" customWidth="1" min="2" max="2"/>
     <col width="15" customWidth="1" min="3" max="3"/>
     <col width="18" customWidth="1" min="4" max="4"/>
     <col width="20" customWidth="1" min="5" max="5"/>
-    <col width="40" customWidth="1" min="6" max="6"/>
+    <col width="45" customWidth="1" min="6" max="6"/>
     <col width="12" customWidth="1" min="7" max="7"/>
     <col width="12" customWidth="1" min="8" max="8"/>
     <col width="12" customWidth="1" min="9" max="9"/>
@@ -500,13 +500,14 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="30" customHeight="1">
+    <row r="2" ht="45" customHeight="1">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>WESTSIDE Sjr Zion, Survey</t>
+          <t>WESTSIDE
+Sjr Zion, Survey</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr">
@@ -526,7 +527,9 @@
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>996211, 300980061004, 300988526002, 300992658003, 600000562, 300922355001, 300989351001</t>
+          <t>996211, 62052000, 62052000
+62046200, 48194000, 33072000
+39264099</t>
         </is>
       </c>
       <c r="G2" s="3" t="inlineStr">
@@ -555,13 +558,14 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="30" customHeight="1">
+    <row r="3" ht="45" customHeight="1">
       <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>SONOVISION ELECTRONICS PVT LTD</t>
+          <t>SONOVISION
+ELECTRONICS PVT LTD</t>
         </is>
       </c>
       <c r="C3" s="3" t="inlineStr">
@@ -581,7 +585,7 @@
       </c>
       <c r="F3" s="2" t="inlineStr">
         <is>
-          <t>85287219, 0</t>
+          <t>85287219</t>
         </is>
       </c>
       <c r="G3" s="3" t="inlineStr">
@@ -610,13 +614,14 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="30" customHeight="1">
+    <row r="4" ht="45" customHeight="1">
       <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>LAKSHMI AGENCIES No:18, Kannadasan Nagar Main Road, Ramapuram</t>
+          <t>LAKSHMI
+AGENCIES</t>
         </is>
       </c>
       <c r="C4" s="3" t="inlineStr">
@@ -636,7 +641,8 @@
       </c>
       <c r="F4" s="2" t="inlineStr">
         <is>
-          <t>15121910, 15121910, 15121910, 15180039, 15180039</t>
+          <t>15121910, 15121910, 15121910
+15180039, 15180039</t>
         </is>
       </c>
       <c r="G4" s="3" t="inlineStr">
@@ -656,7 +662,7 @@
       </c>
       <c r="J4" s="3" t="inlineStr">
         <is>
-          <t>1913.39</t>
+          <t>1506.70</t>
         </is>
       </c>
       <c r="K4" s="3" t="inlineStr">

</xml_diff>

<commit_message>
Improve Excel report presentation by properly aligning multi-line text
Adjust Excel cell formatting to handle multi-line shop names and HSN codes, ensuring proper alignment and row height calculation for better readability.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: a28a4f51-f475-4328-a54d-afd84476b9d9
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/a76d741b-8ad6-464e-a09a-fc6953be1e99/a28a4f51-f475-4328-a54d-afd84476b9d9/COGST8L
</commit_message>
<xml_diff>
--- a/python_backend/output/Consolidated_Invoices_Output.xlsx
+++ b/python_backend/output/Consolidated_Invoices_Output.xlsx
@@ -46,16 +46,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -422,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,57 +441,57 @@
   </cols>
   <sheetData>
     <row r="1" ht="25" customHeight="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>S.No.</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Vendor/Shop Name</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>GSTIN</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Invoice No.</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>HSN Codes</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>CGST</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>SGST</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>IGST</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Total Tax</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Taxable Amount</t>
         </is>
@@ -506,55 +503,53 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>WESTSIDE
-Sjr Zion, Survey</t>
-        </is>
-      </c>
-      <c r="C2" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-28</t>
-        </is>
-      </c>
-      <c r="D2" s="3" t="inlineStr">
-        <is>
-          <t>29AAACL1838J1ZC</t>
-        </is>
-      </c>
-      <c r="E2" s="3" t="inlineStr">
-        <is>
-          <t>W089 100169940</t>
+          <t>SONOVISION
+ELECTRONICS PVT LTD</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>17/Feb/2023</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>37ABCCS7530B1ZK</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>NDYL 3826</t>
         </is>
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>996211, 62052000, 62052000
-62046200, 48194000, 33072000
-39264099</t>
-        </is>
-      </c>
-      <c r="G2" s="3" t="inlineStr">
-        <is>
-          <t>173.91</t>
-        </is>
-      </c>
-      <c r="H2" s="3" t="inlineStr">
-        <is>
-          <t>173.91</t>
-        </is>
-      </c>
-      <c r="I2" s="3" t="inlineStr">
+          <t>85287219</t>
+        </is>
+      </c>
+      <c r="G2" s="1" t="inlineStr">
+        <is>
+          <t>7547</t>
+        </is>
+      </c>
+      <c r="H2" s="1" t="inlineStr">
+        <is>
+          <t>7547</t>
+        </is>
+      </c>
+      <c r="I2" s="1" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="J2" s="3" t="inlineStr">
-        <is>
-          <t>173.91</t>
-        </is>
-      </c>
-      <c r="K2" s="3" t="inlineStr">
-        <is>
-          <t>4045.01</t>
+      <c r="J2" s="1" t="inlineStr">
+        <is>
+          <t>15094</t>
+        </is>
+      </c>
+      <c r="K2" s="1" t="inlineStr">
+        <is>
+          <t>69000</t>
         </is>
       </c>
     </row>
@@ -564,53 +559,54 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>SONOVISION
-ELECTRONICS PVT LTD</t>
-        </is>
-      </c>
-      <c r="C3" s="3" t="inlineStr">
-        <is>
-          <t>17/Feb/2023</t>
-        </is>
-      </c>
-      <c r="D3" s="3" t="inlineStr">
-        <is>
-          <t>37ABCCS7530B1ZK</t>
-        </is>
-      </c>
-      <c r="E3" s="3" t="inlineStr">
-        <is>
-          <t>NDYL 3826</t>
+          <t>LAKSHMI
+AGENCIES</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>17/07/2025</t>
+        </is>
+      </c>
+      <c r="D3" s="1" t="inlineStr">
+        <is>
+          <t>33AABFL7718B1ZQ</t>
+        </is>
+      </c>
+      <c r="E3" s="1" t="inlineStr">
+        <is>
+          <t>LA226412507098</t>
         </is>
       </c>
       <c r="F3" s="2" t="inlineStr">
         <is>
-          <t>85287219</t>
-        </is>
-      </c>
-      <c r="G3" s="3" t="inlineStr">
-        <is>
-          <t>7547</t>
-        </is>
-      </c>
-      <c r="H3" s="3" t="inlineStr">
-        <is>
-          <t>7547</t>
-        </is>
-      </c>
-      <c r="I3" s="3" t="inlineStr">
+          <t>15121910, 15121910, 15121910
+15180039, 15180039</t>
+        </is>
+      </c>
+      <c r="G3" s="1" t="inlineStr">
+        <is>
+          <t>720.00</t>
+        </is>
+      </c>
+      <c r="H3" s="1" t="inlineStr">
+        <is>
+          <t>720.00</t>
+        </is>
+      </c>
+      <c r="I3" s="1" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="J3" s="3" t="inlineStr">
-        <is>
-          <t>15094</t>
-        </is>
-      </c>
-      <c r="K3" s="3" t="inlineStr">
-        <is>
-          <t>69000</t>
+      <c r="J3" s="1" t="inlineStr">
+        <is>
+          <t>1440</t>
+        </is>
+      </c>
+      <c r="K3" s="1" t="inlineStr">
+        <is>
+          <t>33725.00</t>
         </is>
       </c>
     </row>
@@ -620,54 +616,227 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>LAKSHMI
-AGENCIES</t>
-        </is>
-      </c>
-      <c r="C4" s="3" t="inlineStr">
-        <is>
-          <t>17/07/2025</t>
-        </is>
-      </c>
-      <c r="D4" s="3" t="inlineStr">
-        <is>
-          <t>33AABFL7718B1ZQ</t>
-        </is>
-      </c>
-      <c r="E4" s="3" t="inlineStr">
-        <is>
-          <t>LA226412507098</t>
+          <t>WESTSIDE
+Sjr Zion, Survey</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>2024-09-28</t>
+        </is>
+      </c>
+      <c r="D4" s="1" t="inlineStr">
+        <is>
+          <t>29AAACL1838J1ZC</t>
+        </is>
+      </c>
+      <c r="E4" s="1" t="inlineStr">
+        <is>
+          <t>W089 100169940</t>
         </is>
       </c>
       <c r="F4" s="2" t="inlineStr">
         <is>
-          <t>15121910, 15121910, 15121910
-15180039, 15180039</t>
-        </is>
-      </c>
-      <c r="G4" s="3" t="inlineStr">
-        <is>
-          <t>720.00</t>
-        </is>
-      </c>
-      <c r="H4" s="3" t="inlineStr">
-        <is>
-          <t>720.00</t>
-        </is>
-      </c>
-      <c r="I4" s="3" t="inlineStr">
+          <t>996211, 62052000, 62052000
+62046200, 48194000, 33072000
+39264099</t>
+        </is>
+      </c>
+      <c r="G4" s="1" t="inlineStr">
+        <is>
+          <t>173.91</t>
+        </is>
+      </c>
+      <c r="H4" s="1" t="inlineStr">
+        <is>
+          <t>173.91</t>
+        </is>
+      </c>
+      <c r="I4" s="1" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="J4" s="3" t="inlineStr">
-        <is>
-          <t>1506.70</t>
-        </is>
-      </c>
-      <c r="K4" s="3" t="inlineStr">
-        <is>
-          <t>33725.00</t>
+      <c r="J4" s="1" t="inlineStr">
+        <is>
+          <t>173.91</t>
+        </is>
+      </c>
+      <c r="K4" s="1" t="inlineStr">
+        <is>
+          <t>4045.01</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="30" customHeight="1">
+      <c r="A5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>Daniel store</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>25/07/2025</t>
+        </is>
+      </c>
+      <c r="D5" s="1" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E5" s="1" t="inlineStr">
+        <is>
+          <t>IN10830126010369</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="inlineStr">
+        <is>
+          <t>21031000</t>
+        </is>
+      </c>
+      <c r="G5" s="1" t="inlineStr">
+        <is>
+          <t>7.23</t>
+        </is>
+      </c>
+      <c r="H5" s="1" t="inlineStr">
+        <is>
+          <t>7.23</t>
+        </is>
+      </c>
+      <c r="I5" s="1" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J5" s="1" t="inlineStr">
+        <is>
+          <t>14.40</t>
+        </is>
+      </c>
+      <c r="K5" s="1" t="inlineStr">
+        <is>
+          <t>135.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="45" customHeight="1">
+      <c r="A6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>DANIEL STORES
+SUPER MARKET</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>18/07/2025</t>
+        </is>
+      </c>
+      <c r="D6" s="1" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E6" s="1" t="inlineStr">
+        <is>
+          <t>E 16351-</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="inlineStr">
+        <is>
+          <t>18063200, 18063100, 18063100
+18063200, 18063200, 18063200
+18063200, 18063200, 18063200
+18063200, 18063200, 18063200
+19053100, 19053100</t>
+        </is>
+      </c>
+      <c r="G6" s="1" t="inlineStr">
+        <is>
+          <t>484.27</t>
+        </is>
+      </c>
+      <c r="H6" s="1" t="inlineStr">
+        <is>
+          <t>484.27</t>
+        </is>
+      </c>
+      <c r="I6" s="1" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J6" s="1" t="inlineStr">
+        <is>
+          <t>968.54</t>
+        </is>
+      </c>
+      <c r="K6" s="1" t="inlineStr">
+        <is>
+          <t>6099.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="30" customHeight="1">
+      <c r="A7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>Daniel store</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>25/07/2025</t>
+        </is>
+      </c>
+      <c r="D7" s="1" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E7" s="1" t="inlineStr">
+        <is>
+          <t>IN10830126010368</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="inlineStr">
+        <is>
+          <t>09023020, 09023020, 09023020
+09023020, 09021090, 09021090
+21011110, 09023020</t>
+        </is>
+      </c>
+      <c r="G7" s="1" t="inlineStr">
+        <is>
+          <t>212.10</t>
+        </is>
+      </c>
+      <c r="H7" s="1" t="inlineStr">
+        <is>
+          <t>212.10</t>
+        </is>
+      </c>
+      <c r="I7" s="1" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J7" s="1" t="inlineStr">
+        <is>
+          <t>424.20</t>
+        </is>
+      </c>
+      <c r="K7" s="1" t="inlineStr">
+        <is>
+          <t>7069.00</t>
         </is>
       </c>
     </row>

</xml_diff>